<commit_message>
se continua la transaccion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/registro.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/registro.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>pruebasqa99</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>423698529</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>pruebasqa90</t>
   </si>
 </sst>
 </file>
@@ -489,7 +501,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -594,14 +606,59 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="15" spans="1:14">
       <c r="M15" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
+    <hyperlink ref="N3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambio a rama regsitro
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/registro.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/registro.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -104,13 +104,31 @@
   </si>
   <si>
     <t>pruebasqa90</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>95400152</t>
+  </si>
+  <si>
+    <t>sandrita69</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>0370</t>
+  </si>
+  <si>
+    <t>Alterno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +147,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -193,6 +218,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -501,7 +527,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -582,7 +608,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>15</v>
@@ -648,6 +674,44 @@
       </c>
       <c r="N3" s="9" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -660,5 +724,17 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Listas!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G4:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>